<commit_message>
PUB add uncommited results and experiments
</commit_message>
<xml_diff>
--- a/experiments/analysis/results_ifeval_performance.xlsx
+++ b/experiments/analysis/results_ifeval_performance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5653846153846154</v>
+        <v>0.55</v>
       </c>
       <c r="C2" t="n">
         <v>0.5692307692307692</v>
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5</v>
+        <v>0.4846153846153846</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4692307692307692</v>
+        <v>0.4576923076923077</v>
       </c>
     </row>
     <row r="4">
@@ -486,19 +486,32 @@
         <v>0.6076923076923076</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6269230769230769</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>c-FUDGE</t>
+          <t>WildguardCTG</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0.5576923076923077</v>
       </c>
       <c r="C5" t="n">
+        <v>0.6115384615384616</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>c-FUDGE</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.5615384615384615</v>
+      </c>
+      <c r="C6" t="n">
         <v>0.5384615384615384</v>
       </c>
     </row>

</xml_diff>